<commit_message>
Auto-committed on 2023/04/07 週五 17:18:33.96
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L6-共同作業/AcAcctCheck.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L6-共同作業/AcAcctCheck.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\SKL\DB\GenTables\L6-共同作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17240" windowHeight="6290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -180,10 +180,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>業務檔餘額</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>AcctCode</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -352,6 +348,18 @@
   </si>
   <si>
     <t>核心貸方金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>業務檔餘額</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>業務檔已銷金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MasterClsAmt</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -542,7 +550,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -558,10 +566,10 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -573,9 +581,6 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -588,9 +593,6 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -651,8 +653,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -971,111 +982,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.54296875" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.1796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="21.453125" style="7"/>
+    <col min="1" max="1" width="5.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.6640625" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="21.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="39"/>
       <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.4">
-      <c r="A3" s="40" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="37" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="40" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="37" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="37" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="D7" s="12"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1094,460 +1105,481 @@
       <c r="F8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="16">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="30">
+        <v>8</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>2</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="30">
+        <v>4</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>3</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="30">
+        <v>3</v>
+      </c>
+      <c r="F11" s="31"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>4</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="14">
+        <v>3</v>
+      </c>
+      <c r="F12" s="31"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>5</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="32">
+      <c r="D13" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="32">
+        <v>3</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="23"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="32">
+        <v>20</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>7</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="30">
+        <v>18</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
         <v>8</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="16">
+      <c r="B16" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="30">
+        <v>8</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>9</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="30">
+        <v>8</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>10</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="30">
+        <v>8</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>11</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="30">
+        <v>8</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>12</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="30">
+        <v>18</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>13</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="30">
+        <v>18</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>14</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="30">
+        <v>18</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>15</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="30">
+        <v>18</v>
+      </c>
+      <c r="F23" s="30">
         <v>2</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="31" t="s">
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>16</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="30">
+        <v>18</v>
+      </c>
+      <c r="F24" s="30">
+        <v>2</v>
+      </c>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>17</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="30">
+        <v>18</v>
+      </c>
+      <c r="F25" s="30">
+        <v>2</v>
+      </c>
+      <c r="G25" s="27"/>
+    </row>
+    <row r="26" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <v>18</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="30">
+        <v>18</v>
+      </c>
+      <c r="F26" s="30">
+        <v>2</v>
+      </c>
+      <c r="G26" s="27"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>19</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="30">
+        <v>18</v>
+      </c>
+      <c r="F27" s="30">
+        <v>2</v>
+      </c>
+      <c r="G27" s="27"/>
+    </row>
+    <row r="28" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>20</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="35">
+        <v>18</v>
+      </c>
+      <c r="F28" s="35">
+        <v>2</v>
+      </c>
+      <c r="G28" s="36"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>21</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="32">
-        <v>4</v>
-      </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="16">
-        <v>3</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="31" t="s">
+      <c r="E29" s="33">
+        <v>6</v>
+      </c>
+      <c r="F29" s="33"/>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>22</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>23</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="32">
-        <v>3</v>
-      </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="16">
-        <v>4</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="16">
-        <v>3</v>
-      </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="16">
-        <v>5</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="34">
-        <v>3</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="16">
+      <c r="E31" s="33">
         <v>6</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="34">
-        <v>20</v>
-      </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="25"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="16">
-        <v>7</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="32">
-        <v>18</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="16">
-        <v>8</v>
-      </c>
-      <c r="B16" s="22" t="s">
+      <c r="F31" s="33"/>
+      <c r="G31" s="27"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
         <v>24</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="32">
-        <v>8</v>
-      </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="16">
-        <v>9</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="32">
-        <v>8</v>
-      </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="16">
-        <v>10</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="32">
-        <v>8</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="16">
-        <v>11</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="32">
-        <v>8</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="16">
-        <v>12</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="32">
-        <v>18</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="16">
-        <v>13</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="32">
-        <v>18</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="23"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="16">
-        <v>14</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="32">
-        <v>18</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="16">
-        <v>15</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="32">
-        <v>18</v>
-      </c>
-      <c r="F23" s="36">
-        <v>2</v>
-      </c>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="16">
-        <v>16</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="32">
-        <v>18</v>
-      </c>
-      <c r="F24" s="36">
-        <v>2</v>
-      </c>
-      <c r="G24" s="26"/>
-    </row>
-    <row r="25" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="16">
-        <v>17</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="32">
-        <v>18</v>
-      </c>
-      <c r="F25" s="36">
-        <v>2</v>
-      </c>
-      <c r="G25" s="29"/>
-    </row>
-    <row r="26" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="16">
-        <v>18</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="32">
-        <v>18</v>
-      </c>
-      <c r="F26" s="36">
-        <v>2</v>
-      </c>
-      <c r="G26" s="29"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="16">
-        <v>19</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="32">
-        <v>18</v>
-      </c>
-      <c r="F27" s="36">
-        <v>2</v>
-      </c>
-      <c r="G27" s="29"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="16">
-        <v>20</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="35">
-        <v>6</v>
-      </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="27"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="16">
-        <v>21</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="26" t="s">
+      <c r="B32" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="26"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="16">
-        <v>22</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="35">
-        <v>6</v>
-      </c>
-      <c r="F30" s="35"/>
-      <c r="G30" s="29"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" s="16">
-        <v>23</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="29"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1577,15 +1609,15 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="71.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="71.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1596,15 +1628,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1622,33 +1654,33 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.90625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="30" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>